<commit_message>
chore(doc): add status column to example
</commit_message>
<xml_diff>
--- a/schema/example.xlsx
+++ b/schema/example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t xml:space="preserve">Broadcast Title</t>
   </si>
@@ -30,6 +30,9 @@
   </si>
   <si>
     <t xml:space="preserve">Genre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft</t>
   </si>
   <si>
     <t xml:space="preserve">Mon</t>
@@ -328,10 +331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -339,8 +342,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="2" width="6.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="2" width="6.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,7 +357,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -373,68 +377,74 @@
       </c>
       <c r="J1" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>